<commit_message>
many other changes. Will have to create a very big notebook to be able to do everything in one, it is being a mess
</commit_message>
<xml_diff>
--- a/portfolio-optimization/results/bench_vs_portfolio.xlsx
+++ b/portfolio-optimization/results/bench_vs_portfolio.xlsx
@@ -472,22 +472,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.0005437115550206588</v>
+        <v>0.0005620882150452121</v>
       </c>
       <c r="C2" t="n">
-        <v>0.004744438861753729</v>
+        <v>0.004717853727405196</v>
       </c>
       <c r="D2" t="n">
-        <v>2.250970011291903e-05</v>
+        <v>2.225814379319111e-05</v>
       </c>
       <c r="E2" t="n">
-        <v>0.137015311865206</v>
+        <v>0.1416462301913934</v>
       </c>
       <c r="F2" t="n">
-        <v>0.07531563203250434</v>
+        <v>0.07489360610815958</v>
       </c>
       <c r="G2" t="n">
-        <v>1.229695739992404</v>
+        <v>1.29845837641938</v>
       </c>
     </row>
     <row r="3">
@@ -497,22 +497,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.0002330403864534556</v>
+        <v>0.0002540042595312843</v>
       </c>
       <c r="C3" t="n">
-        <v>0.004839415689665924</v>
+        <v>0.004812597344483673</v>
       </c>
       <c r="D3" t="n">
-        <v>2.341994421738471e-05</v>
+        <v>2.316109320013131e-05</v>
       </c>
       <c r="E3" t="n">
-        <v>0.05872617738627081</v>
+        <v>0.06400907340188365</v>
       </c>
       <c r="F3" t="n">
-        <v>0.07682334243432101</v>
+        <v>0.07639761440276188</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1864820890671187</v>
+        <v>0.2566712790075648</v>
       </c>
     </row>
   </sheetData>

</xml_diff>